<commit_message>
Remove model-level implementation from main
</commit_message>
<xml_diff>
--- a/cave.xlsx
+++ b/cave.xlsx
@@ -12,7 +12,7 @@
     <sheet name="L2" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="L3" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="L4" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Characters" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="C" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t xml:space="preserve">P</t>
   </si>
@@ -133,10 +133,10 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+      <selection pane="topLeft" activeCell="N18" activeCellId="0" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -2085,10 +2085,10 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
+      <selection pane="topLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -4037,10 +4037,10 @@
   <dimension ref="A1:Y25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -5992,7 +5992,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
   </cols>
@@ -7938,13 +7938,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -7974,27 +7974,44 @@
         <v>336</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>61</v>
+        <v>125</v>
       </c>
       <c r="E2" s="0" t="n">
         <v>336</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="D3" s="0" t="n">
         <v>200</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>90</v>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>110</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>240</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>